<commit_message>
Update Algo Comparison Table
</commit_message>
<xml_diff>
--- a/AlgoComparisonTable.xlsx
+++ b/AlgoComparisonTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\Breast-Cancer-Diagnostics-using-Classification-Algorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Projects\Github Projects\Breast-Cancer-Diagnostics-using-Classification-Algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{ABEE58CA-45FE-4558-955D-23D7E61EDA0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3BB619-FC85-46F3-A563-8341AC604F41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1740" windowWidth="21600" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison List" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Comparison List</t>
   </si>
@@ -46,21 +46,6 @@
     <t>Xception</t>
   </si>
   <si>
-    <t>Resnet</t>
-  </si>
-  <si>
-    <t>Inception</t>
-  </si>
-  <si>
-    <t>InceptionResnetV3</t>
-  </si>
-  <si>
-    <t>Magnification Classification</t>
-  </si>
-  <si>
-    <t>Tumor Class Classification</t>
-  </si>
-  <si>
     <t>B+40X</t>
   </si>
   <si>
@@ -83,6 +68,81 @@
   </si>
   <si>
     <t>M+400X</t>
+  </si>
+  <si>
+    <t>40x+B/M</t>
+  </si>
+  <si>
+    <t>200x+B/M</t>
+  </si>
+  <si>
+    <t>400x+B/M</t>
+  </si>
+  <si>
+    <t>100x+B/M</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Class. -&gt;</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Mag.-&gt;</t>
+  </si>
+  <si>
+    <t>Magnification</t>
+  </si>
+  <si>
+    <t>B-&gt;</t>
+  </si>
+  <si>
+    <t>Benign</t>
+  </si>
+  <si>
+    <t>M.-&gt;</t>
+  </si>
+  <si>
+    <t>Malignant</t>
+  </si>
+  <si>
+    <t>Magnifiaction</t>
+  </si>
+  <si>
+    <t>40X</t>
+  </si>
+  <si>
+    <t>100X</t>
+  </si>
+  <si>
+    <t>200X</t>
+  </si>
+  <si>
+    <t>400X</t>
+  </si>
+  <si>
+    <t>Tumor Class. using Mag. Class.</t>
+  </si>
+  <si>
+    <t>Mag. Class.</t>
+  </si>
+  <si>
+    <t>Benign Sub-Class. using Tumor &amp; Mag. Class.</t>
+  </si>
+  <si>
+    <t>Malignant Sub-Class. using Tumor &amp; Mag. Class.</t>
+  </si>
+  <si>
+    <t>ResNet50</t>
+  </si>
+  <si>
+    <t>InceptionV3</t>
+  </si>
+  <si>
+    <t>InceptionResnetV2</t>
   </si>
 </sst>
 </file>
@@ -155,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -183,6 +243,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0">
@@ -193,11 +347,23 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1">
@@ -206,22 +372,40 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -230,7 +414,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <vertical/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -263,9 +476,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Table Comparison " defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Comparison " pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="2"/>
-      <tableStyleElement type="headerRow" dxfId="1"/>
-      <tableStyleElement type="firstColumn" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -280,20 +493,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Comparison" displayName="Comparison" ref="B3:G7" headerRowCellStyle="Normal">
-  <autoFilter ref="B3:G7" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Comparison" displayName="Comparison" ref="B3:J7" headerRowCellStyle="Normal">
+  <autoFilter ref="B3:J7" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="6">
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Deep Learning/Machine Learning" totalsRowLabel="Total" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Magnification Classification" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Tumor Class Classification" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="B+40X" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mag. Class." dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="40x+B/M" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{9AE58507-248D-43F9-A27A-39A1B95A1EE2}" name="100x+B/M"/>
+    <tableColumn id="8" xr3:uid="{1A1ECEFD-27DE-4A12-A445-F749BBCB424C}" name="200x+B/M"/>
+    <tableColumn id="7" xr3:uid="{0FF71547-B37C-4CDC-BD36-63E6E48BC4AF}" name="400x+B/M"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="B+40X" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="B+100X" dataCellStyle="Normal"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="B+200X" totalsRowFunction="count" dataCellStyle="Normal"/>
   </tableColumns>
@@ -573,10 +792,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L9"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -584,282 +803,421 @@
     <col min="1" max="1" width="3.25" customWidth="1"/>
     <col min="2" max="2" width="23.75" customWidth="1"/>
     <col min="3" max="3" width="16.125" customWidth="1"/>
-    <col min="4" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="12" width="12.625" customWidth="1"/>
+    <col min="4" max="7" width="14.75" customWidth="1"/>
+    <col min="8" max="15" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="2:12" ht="10.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="2:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="13"/>
+    </row>
+    <row r="3" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="L3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="M3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="N3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="O3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="9" t="s">
+    </row>
+    <row r="4" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="17">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="15">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="17">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="17">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="12">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="17">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="12">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
-      <c r="J4" s="4">
-        <v>0</v>
-      </c>
-      <c r="K4" s="4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7">
-        <v>0</v>
-      </c>
-      <c r="D5" s="7">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7">
-        <v>0</v>
-      </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7">
-        <v>0</v>
-      </c>
-      <c r="K7" s="7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7">
-        <v>0</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="H8" s="7">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7">
-        <v>0</v>
-      </c>
-      <c r="K8" s="7">
-        <v>0</v>
-      </c>
-      <c r="L8" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <v>0</v>
-      </c>
-      <c r="K9" s="4">
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <dataValidations disablePrompts="1" xWindow="425" yWindow="315" count="7">
+  <dataValidations xWindow="425" yWindow="315" count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Comparison List in this worksheet. Enter data in Comparison table" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter item details in table below" sqref="B1:C1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Subject/Item in this column under this heading" sqref="B3" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Feature name in this cell and description in this column under this heading" sqref="C3:E3 I3" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Ranking in this column under this heading" sqref="F3 J3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter notes in this column under this heading" sqref="G4:H4 K4:L4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="G3:H3 K3:L3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Feature name in this cell and description in this column under this heading" sqref="L3 C3:H3 E14:G14" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Ranking in this column under this heading" sqref="I3 M3 H14" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter notes in this column under this heading" sqref="J4:K4 N4:O4 I15:J15" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="J3:K3 N3:O3 I14:J14" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="69" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>